<commit_message>
Added a commmnet in Aims Lab
</commit_message>
<xml_diff>
--- a/Aims Lab.xlsx
+++ b/Aims Lab.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="135">
   <si>
     <t>Date</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>ATS</t>
+  </si>
+  <si>
+    <t>IPD Bill not Recived</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
   <dimension ref="A1:J191"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="I162" sqref="I162"/>
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2800,6 +2803,9 @@
       </c>
       <c r="E139" s="2">
         <v>490</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="140" spans="1:8">

</xml_diff>